<commit_message>
added events insertion functionality
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C2" t="n">
         <v>9</v>
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C3" t="n">
         <v>22</v>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C4" t="n">
         <v>20</v>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C5" t="n">
         <v>13</v>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C7" t="n">
         <v>128</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="C8" t="n">
         <v>128</v>
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C9" t="n">
         <v>128</v>
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C10" t="n">
         <v>128</v>
@@ -774,7 +774,7 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C11" t="n">
         <v>128</v>
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C12" t="n">
         <v>5</v>
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C13" t="n">
         <v>24</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="C14" t="n">
         <v>45</v>
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="C15" t="n">
         <v>45</v>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="C16" t="n">
         <v>45</v>
@@ -966,7 +966,7 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="C17" t="n">
         <v>26</v>
@@ -998,7 +998,7 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="C18" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
standardised units to minutes and pomodoro column fixed
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,30 +450,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Minutes</t>
+          <t>Study Block (Minutes)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Study Block (Minutes)</t>
+          <t>Study Block Summation (Minutes)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Study Block Summation (Minutes)</t>
+          <t>Pomodoro Session</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Pomodoro Session</t>
+          <t>Start Time</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Start Time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
@@ -486,7 +481,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C2" t="n">
         <v>9</v>
@@ -495,20 +490,13 @@
         <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>44593.58333333334</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>44593.60416666666</v>
       </c>
     </row>
     <row r="3">
@@ -518,189 +506,147 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C3" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E3" t="n">
-        <v>31</v>
-      </c>
-      <c r="F3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+      <c r="F3" s="2" t="n">
+        <v>44593.58333333334</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>44593.60416666666</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Setup Kubernetes</t>
+          <t>Kubernetes Overview</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E4" t="n">
-        <v>50.99999999999999</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>44593.60416666666</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>44593.625</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kubernetes Concepts</t>
+          <t>Setup Kubernetes</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E5" t="n">
-        <v>63.99999999999999</v>
-      </c>
-      <c r="F5" t="n">
         <v>2</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>14:30:00</t>
-        </is>
+      <c r="F5" s="2" t="n">
+        <v>44593.60416666666</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>44593.625</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>YAML Introduction</t>
+          <t>Kubernetes Concepts</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="E6" t="n">
-        <v>71.99999999999999</v>
-      </c>
-      <c r="F6" t="n">
         <v>2</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>14:30:00</t>
-        </is>
+      <c r="F6" s="2" t="n">
+        <v>44593.60416666666</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>44593.625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
+          <t>Kubernetes Concepts</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C7" t="n">
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="E7" t="n">
-        <v>102</v>
-      </c>
-      <c r="F7" t="n">
         <v>3</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>14:30:00</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>15:00:00</t>
-        </is>
+      <c r="F7" s="2" t="n">
+        <v>44593.625</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>44593.64583333334</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
+          <t>YAML Introduction</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44571</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C8" t="n">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
-        <v>18.00000000000001</v>
+        <v>72</v>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
-      </c>
-      <c r="F8" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>15:00:00</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>15:30:00</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>44593.625</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>44593.64583333334</v>
       </c>
     </row>
     <row r="9">
@@ -710,29 +656,22 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44572</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C9" t="n">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E9" t="n">
-        <v>150</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>44593.625</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>44593.64583333334</v>
       </c>
     </row>
     <row r="10">
@@ -742,29 +681,22 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44572</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C10" t="n">
-        <v>128</v>
+        <v>12</v>
       </c>
       <c r="D10" t="n">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="E10" t="n">
-        <v>180</v>
-      </c>
-      <c r="F10" t="n">
-        <v>6</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>44593.64583333334</v>
+      </c>
+      <c r="G10" s="2" t="n">
+        <v>44593.66666666666</v>
       </c>
     </row>
     <row r="11">
@@ -774,253 +706,297 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44572</v>
+        <v>44593.58333333334</v>
       </c>
       <c r="C11" t="n">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="D11" t="n">
-        <v>19.99999999999998</v>
+        <v>120</v>
       </c>
       <c r="E11" t="n">
-        <v>200</v>
-      </c>
-      <c r="F11" t="n">
-        <v>6</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>44593.64583333334</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>44593.66666666666</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Networking in Kubernetes</t>
+          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44572</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C12" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" t="n">
+        <v>150</v>
+      </c>
+      <c r="E12" t="n">
         <v>5</v>
       </c>
-      <c r="D12" t="n">
-        <v>5</v>
-      </c>
-      <c r="E12" t="n">
-        <v>205</v>
-      </c>
-      <c r="F12" t="n">
-        <v>6</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+      <c r="F12" s="2" t="n">
+        <v>44594.58333333334</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>44594.60416666666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44572</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C13" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>24</v>
+        <v>180</v>
       </c>
       <c r="E13" t="n">
-        <v>229</v>
-      </c>
-      <c r="F13" t="n">
-        <v>7</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>14:30:00</t>
-        </is>
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>44594.60416666666</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>44594.625</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44572</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C14" t="n">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>11.00000000000001</v>
+        <v>200</v>
       </c>
       <c r="E14" t="n">
-        <v>240</v>
-      </c>
-      <c r="F14" t="n">
-        <v>8</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>14:30:00</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>15:00:00</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>44594.625</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>44594.64583333334</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Networking in Kubernetes</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44573</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C15" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>30</v>
+        <v>205</v>
       </c>
       <c r="E15" t="n">
-        <v>270</v>
-      </c>
-      <c r="F15" t="n">
-        <v>9</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>44594.625</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>44594.64583333334</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44573</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C16" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D16" t="n">
-        <v>3.999999999999986</v>
+        <v>210</v>
       </c>
       <c r="E16" t="n">
-        <v>274</v>
-      </c>
-      <c r="F16" t="n">
-        <v>9</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>44594.625</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>44594.64583333334</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kubernetes on the Cloud</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44573</v>
+        <v>44594.58333333334</v>
       </c>
       <c r="C17" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D17" t="n">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="E17" t="n">
-        <v>300</v>
-      </c>
-      <c r="F17" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+        <v>8</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>44594.64583333334</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>44594.66666666666</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Microservices Architechture</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44594.58333333334</v>
+      </c>
+      <c r="C18" t="n">
+        <v>11</v>
+      </c>
+      <c r="D18" t="n">
+        <v>240</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>44594.64583333334</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>44594.66666666666</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Microservices Architechture</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44595.58333333334</v>
+      </c>
+      <c r="C19" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" t="n">
+        <v>270</v>
+      </c>
+      <c r="E19" t="n">
+        <v>9</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>44595.58333333334</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>44595.60416666666</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Microservices Architechture</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44595.58333333334</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" t="n">
+        <v>274</v>
+      </c>
+      <c r="E20" t="n">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>44595.60416666666</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>44595.625</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Kubernetes on the Cloud</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>44595.58333333334</v>
+      </c>
+      <c r="C21" t="n">
+        <v>26</v>
+      </c>
+      <c r="D21" t="n">
+        <v>300</v>
+      </c>
+      <c r="E21" t="n">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>44595.60416666666</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>44595.625</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>Conclusion</t>
         </is>
       </c>
-      <c r="B18" s="2" t="n">
-        <v>44573</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="B22" s="2" t="n">
+        <v>44595.58333333334</v>
+      </c>
+      <c r="C22" t="n">
         <v>2</v>
       </c>
-      <c r="D18" t="n">
-        <v>2</v>
-      </c>
-      <c r="E18" t="n">
+      <c r="D22" t="n">
         <v>302</v>
       </c>
-      <c r="F18" t="n">
-        <v>10</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
+      <c r="E22" t="n">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>44595.625</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>44595.64583333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned up code in app, created new df for results.xlsx and renamed src-data to sample
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Study Block (Minutes)</t>
+          <t>Minutes</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,6 +471,11 @@
       <c r="G1" s="1" t="inlineStr">
         <is>
           <t>End Time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Break Time</t>
         </is>
       </c>
     </row>
@@ -481,7 +486,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C2" t="n">
         <v>9</v>
@@ -492,11 +497,20 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="n">
-        <v>44593.58333333334</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>44593.60416666666</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -506,7 +520,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C3" t="n">
         <v>21</v>
@@ -517,11 +531,20 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="n">
-        <v>44593.58333333334</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>44593.60416666666</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -531,7 +554,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -542,11 +565,20 @@
       <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="n">
-        <v>44593.60416666666</v>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>44593.625</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -556,7 +588,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C5" t="n">
         <v>20</v>
@@ -567,11 +599,20 @@
       <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>44593.60416666666</v>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>44593.625</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -581,7 +622,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C6" t="n">
         <v>9</v>
@@ -592,11 +633,20 @@
       <c r="E6" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="n">
-        <v>44593.60416666666</v>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>44593.625</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -606,7 +656,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44574.54166666666</v>
       </c>
       <c r="C7" t="n">
         <v>4</v>
@@ -617,11 +667,20 @@
       <c r="E7" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="2" t="n">
-        <v>44593.625</v>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>44593.64583333334</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -631,7 +690,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44574.54166666666</v>
       </c>
       <c r="C8" t="n">
         <v>8</v>
@@ -642,11 +701,20 @@
       <c r="E8" t="n">
         <v>3</v>
       </c>
-      <c r="F8" s="2" t="n">
-        <v>44593.625</v>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>44593.64583333334</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -656,7 +724,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44574.54166666666</v>
       </c>
       <c r="C9" t="n">
         <v>18</v>
@@ -667,11 +735,20 @@
       <c r="E9" t="n">
         <v>3</v>
       </c>
-      <c r="F9" s="2" t="n">
-        <v>44593.625</v>
-      </c>
-      <c r="G9" s="2" t="n">
-        <v>44593.64583333334</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -681,22 +758,31 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44575.54166666666</v>
       </c>
       <c r="C10" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D10" t="n">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="n">
-        <v>44593.64583333334</v>
-      </c>
-      <c r="G10" s="2" t="n">
-        <v>44593.66666666666</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -706,22 +792,31 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44593.58333333334</v>
+        <v>44576.54166666666</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D11" t="n">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>44593.64583333334</v>
-      </c>
-      <c r="G11" s="2" t="n">
-        <v>44593.66666666666</v>
+        <v>5</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -731,22 +826,31 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44577.54166666666</v>
       </c>
       <c r="C12" t="n">
         <v>30</v>
       </c>
       <c r="D12" t="n">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E12" t="n">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>44594.58333333334</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>44594.60416666666</v>
+        <v>6</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -756,72 +860,99 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44578.54166666666</v>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E13" t="n">
-        <v>6</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>44594.60416666666</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>44594.625</v>
+        <v>7</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
+          <t>Networking in Kubernetes</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44578.54166666666</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D14" t="n">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="E14" t="n">
         <v>7</v>
       </c>
-      <c r="F14" s="2" t="n">
-        <v>44594.625</v>
-      </c>
-      <c r="G14" s="2" t="n">
-        <v>44594.64583333334</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Networking in Kubernetes</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44578.54166666666</v>
       </c>
       <c r="C15" t="n">
         <v>5</v>
       </c>
       <c r="D15" t="n">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>44594.625</v>
-      </c>
-      <c r="G15" s="2" t="n">
-        <v>44594.64583333334</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -831,47 +962,65 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44579.54166666666</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D16" t="n">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>44594.625</v>
-      </c>
-      <c r="G16" s="2" t="n">
-        <v>44594.64583333334</v>
+        <v>8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Microservices Architechture</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44579.54166666666</v>
       </c>
       <c r="C17" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="E17" t="n">
         <v>8</v>
       </c>
-      <c r="F17" s="2" t="n">
-        <v>44594.64583333334</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>44594.66666666666</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -881,22 +1030,31 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44594.58333333334</v>
+        <v>44580.54166666666</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>44594.64583333334</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>44594.66666666666</v>
+        <v>9</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -906,97 +1064,99 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44595.58333333334</v>
+        <v>44581.54166666666</v>
       </c>
       <c r="C19" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>44595.58333333334</v>
-      </c>
-      <c r="G19" s="2" t="n">
-        <v>44595.60416666666</v>
+        <v>10</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Kubernetes on the Cloud</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44595.58333333334</v>
+        <v>44581.54166666666</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D20" t="n">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="E20" t="n">
         <v>10</v>
       </c>
-      <c r="F20" s="2" t="n">
-        <v>44595.60416666666</v>
-      </c>
-      <c r="G20" s="2" t="n">
-        <v>44595.625</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kubernetes on the Cloud</t>
+          <t>Conclusion</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44595.58333333334</v>
+        <v>44582.54166666666</v>
       </c>
       <c r="C21" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>44595.60416666666</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>44595.625</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Conclusion</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>44595.58333333334</v>
-      </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
-      <c r="D22" t="n">
-        <v>302</v>
-      </c>
-      <c r="E22" t="n">
         <v>11</v>
       </c>
-      <c r="F22" s="2" t="n">
-        <v>44595.625</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>44595.64583333334</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>13:00:00</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>13:30:00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed print statement and updated result via new pomodor split
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,13 +504,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>44572.58333333334</v>
       </c>
     </row>
     <row r="3">
@@ -523,10 +521,10 @@
         <v>44572.54166666666</v>
       </c>
       <c r="C3" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -538,33 +536,31 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>44572.58333333334</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kubernetes Overview</t>
+          <t>Setup Kubernetes</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C4" t="n">
+        <v>14</v>
+      </c>
+      <c r="D4" t="n">
+        <v>45</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>31</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2</v>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>13:00:00</t>
@@ -572,13 +568,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>44572.58333333334</v>
       </c>
     </row>
     <row r="5">
@@ -588,10 +582,10 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C5" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
         <v>51</v>
@@ -601,18 +595,16 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>44572.625</v>
       </c>
     </row>
     <row r="6">
@@ -622,99 +614,93 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>44572.625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kubernetes Concepts</t>
+          <t>YAML Introduction</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44574.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C7" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>44572.625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>YAML Introduction</t>
+          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44574.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D8" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>44572.625</v>
       </c>
     </row>
     <row r="9">
@@ -724,31 +710,29 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44574.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D9" t="n">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>44572.66666666666</v>
       </c>
     </row>
     <row r="10">
@@ -758,31 +742,29 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44575.54166666666</v>
+        <v>44572.54166666666</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D10" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="E10" t="n">
         <v>4</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>16:00:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>16:45:00</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>44572.70833333334</v>
       </c>
     </row>
     <row r="11">
@@ -792,13 +774,13 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44576.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="E11" t="n">
         <v>5</v>
@@ -810,32 +792,30 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>44573.58333333334</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
+          <t>Networking in Kubernetes</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44577.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C12" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D12" t="n">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -844,32 +824,30 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>44573.58333333334</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44578.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C13" t="n">
         <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="E13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -878,285 +856,171 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>44573.58333333334</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Networking in Kubernetes</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44578.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="E14" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>44573.625</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Microservices Architechture</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44578.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D15" t="n">
-        <v>210</v>
+        <v>270</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>44573.625</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Microservices Architechture</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44579.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>44573.66666666666</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Kubernetes on the Cloud</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44579.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D17" t="n">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>44573.66666666666</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Conclusion</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44580.54166666666</v>
+        <v>44573.54166666666</v>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
-        <v>270</v>
+        <v>302</v>
       </c>
       <c r="E18" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Microservices Architechture</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>44581.54166666666</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4</v>
-      </c>
-      <c r="D19" t="n">
-        <v>274</v>
-      </c>
-      <c r="E19" t="n">
-        <v>10</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Kubernetes on the Cloud</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>44581.54166666666</v>
-      </c>
-      <c r="C20" t="n">
-        <v>26</v>
-      </c>
-      <c r="D20" t="n">
-        <v>300</v>
-      </c>
-      <c r="E20" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Conclusion</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>44582.54166666666</v>
-      </c>
-      <c r="C21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D21" t="n">
-        <v>302</v>
-      </c>
-      <c r="E21" t="n">
-        <v>11</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>13:00:00</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>13:30:00</t>
-        </is>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>44573.66666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated readme and sample-data to src-data
</commit_message>
<xml_diff>
--- a/data/result.xlsx
+++ b/data/result.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C2" t="n">
         <v>9</v>
@@ -507,8 +507,10 @@
           <t>13:45:00</t>
         </is>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>44572.58333333334</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -518,7 +520,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C3" t="n">
         <v>22</v>
@@ -539,8 +541,10 @@
           <t>13:45:00</t>
         </is>
       </c>
-      <c r="H3" s="2" t="n">
-        <v>44572.58333333334</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -550,7 +554,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C4" t="n">
         <v>14</v>
@@ -571,8 +575,10 @@
           <t>13:45:00</t>
         </is>
       </c>
-      <c r="H4" s="2" t="n">
-        <v>44572.58333333334</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -582,7 +588,7 @@
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C5" t="n">
         <v>6</v>
@@ -603,8 +609,10 @@
           <t>14:45:00</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>44572.625</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -614,7 +622,7 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C6" t="n">
         <v>13</v>
@@ -635,8 +643,10 @@
           <t>14:45:00</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>44572.625</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -646,7 +656,7 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
@@ -667,8 +677,10 @@
           <t>14:45:00</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
-        <v>44572.625</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -678,7 +690,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C8" t="n">
         <v>18</v>
@@ -699,8 +711,10 @@
           <t>14:45:00</t>
         </is>
       </c>
-      <c r="H8" s="2" t="n">
-        <v>44572.625</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -710,13 +724,13 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44562</v>
       </c>
       <c r="C9" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
@@ -731,8 +745,10 @@
           <t>15:45:00</t>
         </is>
       </c>
-      <c r="H9" s="2" t="n">
-        <v>44572.66666666666</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>16:00:00</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -742,29 +758,31 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44572.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C10" t="n">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>180</v>
+        <v>135</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>16:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>16:45:00</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>44572.70833333334</v>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -774,93 +792,99 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D11" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>14:00:00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>13:45:00</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>44573.58333333334</v>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Networking in Kubernetes</t>
+          <t>Kubernets Concepts - PODs, ReplicaSets, Deployments</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E12" t="n">
         <v>5</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>13:45:00</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>44573.58333333334</v>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>16:00:00</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Services</t>
+          <t>Networking in Kubernetes</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C13" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="E13" t="n">
         <v>5</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>13:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>13:45:00</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>44573.58333333334</v>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>16:00:00</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -870,61 +894,65 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>15:00:00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>14:45:00</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="n">
-        <v>44573.625</v>
+          <t>15:45:00</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>16:00:00</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Microservices Architechture</t>
+          <t>Services</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C15" t="n">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>270</v>
+        <v>229</v>
       </c>
       <c r="E15" t="n">
         <v>6</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>14:00:00</t>
+          <t>16:00:00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>14:45:00</t>
-        </is>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>44573.625</v>
+          <t>16:45:00</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>17:00:00</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -934,93 +962,167 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44563</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>15:00:00</t>
+          <t>16:00:00</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>15:45:00</t>
-        </is>
-      </c>
-      <c r="H16" s="2" t="n">
-        <v>44573.66666666666</v>
+          <t>16:45:00</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>17:00:00</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kubernetes on the Cloud</t>
+          <t>Microservices Architechture</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44564</v>
       </c>
       <c r="C17" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="E17" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>15:00:00</t>
+          <t>13:00:00</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>15:45:00</t>
-        </is>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>44573.66666666666</v>
+          <t>13:45:00</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Conclusion</t>
+          <t>Microservices Architechture</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44573.54166666666</v>
+        <v>44564</v>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" t="n">
-        <v>302</v>
+        <v>274</v>
       </c>
       <c r="E18" t="n">
         <v>7</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>15:00:00</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>15:45:00</t>
-        </is>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>44573.66666666666</v>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Kubernetes on the Cloud</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44564</v>
+      </c>
+      <c r="C19" t="n">
+        <v>26</v>
+      </c>
+      <c r="D19" t="n">
+        <v>300</v>
+      </c>
+      <c r="E19" t="n">
+        <v>7</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44564</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>302</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>14:45:00</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>15:00:00</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>